<commit_message>
# update schedule.xlsx and add some study file.
</commit_message>
<xml_diff>
--- a/history/drive.xlsx
+++ b/history/drive.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="18180" windowHeight="9900"/>
+    <workbookView xWindow="7590" yWindow="225" windowWidth="18180" windowHeight="9900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="76">
   <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -245,10 +245,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>showa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>公司</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -270,6 +266,58 @@
   </si>
   <si>
     <t>kaine,simon,沈家亮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:30-18:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8:50-9:20 AM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:30-18:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sam,Simon,Kaine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sam,Simon,Kaine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:30-19:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>东英羽毛球馆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20:30-21:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Merring,angel,sue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:40-18:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>岑村红花岗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9:05-9:40 AM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sam,Simon,Kaine</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -623,15 +671,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30:F32"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
@@ -1106,7 +1157,7 @@
         <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1157,16 +1208,16 @@
         <v>13</v>
       </c>
       <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
         <v>57</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>58</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1186,7 +1237,7 @@
         <v>5</v>
       </c>
       <c r="F27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1206,7 +1257,7 @@
         <v>43</v>
       </c>
       <c r="F28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1226,24 +1277,24 @@
         <v>5</v>
       </c>
       <c r="F29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="1">
-        <v>40824</v>
+        <v>40823</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
         <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F30" t="s">
         <v>23</v>
@@ -1254,16 +1305,16 @@
         <v>40824</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
         <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E31" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="F31" t="s">
         <v>23</v>
@@ -1274,19 +1325,342 @@
         <v>40824</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
         <v>13</v>
       </c>
       <c r="D32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" t="s">
         <v>43</v>
-      </c>
-      <c r="E32" t="s">
-        <v>5</v>
       </c>
       <c r="F32" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1">
+        <v>40824</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="1">
+        <v>40824</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="1">
+        <v>40826</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="1">
+        <v>40826</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="1">
+        <v>40826</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="1">
+        <v>40826</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="1">
+        <v>40827</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="1">
+        <v>40827</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="1">
+        <v>40828</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="1">
+        <v>40828</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" t="s">
+        <v>69</v>
+      </c>
+      <c r="F42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="1">
+        <v>40828</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="1">
+        <v>40829</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="1">
+        <v>40829</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" t="s">
+        <v>43</v>
+      </c>
+      <c r="F45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="1">
+        <v>40829</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" t="s">
+        <v>5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="1">
+        <v>40829</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" t="s">
+        <v>73</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="1">
+        <v>40830</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
# update cash_hist.xls .
</commit_message>
<xml_diff>
--- a/history/drive.xlsx
+++ b/history/drive.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="179">
   <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -628,10 +628,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>6:30-9:00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>actavis</t>
   </si>
   <si>
@@ -639,7 +635,120 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>17:30-20:00</t>
+    <t>13:00-13:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:30-18:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:30-18:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英东羽毛球馆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20:30-21:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+油 ￥200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+油 ￥140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6:30-8:50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>副驾座把手被拉断</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12:25-12:50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHOWA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:50-18:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>09:00-9:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>08:40-9:20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:50-18:20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8:50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-9:20</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:30-21:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20:30-23:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公司</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -647,6 +756,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -686,7 +798,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -697,6 +809,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -993,21 +1111,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H122"/>
+  <dimension ref="A1:H140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D120" sqref="D120"/>
+      <selection pane="bottomRight" activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
@@ -1015,7 +1133,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1038,7 +1156,7 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="1">
+      <c r="A2" s="4">
         <v>40744</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1058,7 +1176,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="1">
+      <c r="A3" s="4">
         <v>40756</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1078,7 +1196,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="1">
+      <c r="A4" s="4">
         <v>40759</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1098,7 +1216,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="1">
+      <c r="A5" s="4">
         <v>40760</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1118,7 +1236,7 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="1">
+      <c r="A6" s="4">
         <v>40778</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1138,7 +1256,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="1">
+      <c r="A7" s="4">
         <v>40778</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1158,7 +1276,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="1">
+      <c r="A8" s="4">
         <v>40779</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1181,7 +1299,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="1">
+      <c r="A9" s="4">
         <v>40779</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1204,7 +1322,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="1">
+      <c r="A10" s="4">
         <v>40780</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1224,7 +1342,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="1">
+      <c r="A11" s="4">
         <v>40780</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1247,7 +1365,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="1">
+      <c r="A12" s="4">
         <v>40785</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1267,7 +1385,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="1">
+      <c r="A13" s="4">
         <v>40785</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1287,7 +1405,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="1">
+      <c r="A14" s="4">
         <v>40786</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1307,7 +1425,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="1">
+      <c r="A15" s="4">
         <v>40801</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1327,7 +1445,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="1">
+      <c r="A16" s="4">
         <v>40801</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1347,7 +1465,7 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="1">
+      <c r="A17" s="4">
         <v>40802</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1367,7 +1485,7 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="1">
+      <c r="A18" s="4">
         <v>40802</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1387,7 +1505,7 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="1">
+      <c r="A19" s="4">
         <v>40802</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1407,7 +1525,7 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="1">
+      <c r="A20" s="4">
         <v>40802</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1427,7 +1545,7 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="1">
+      <c r="A21" s="4">
         <v>40803</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1447,7 +1565,7 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="1">
+      <c r="A22" s="4">
         <v>40803</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1467,7 +1585,7 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="1">
+      <c r="A23" s="4">
         <v>40804</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1487,7 +1605,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="1">
+      <c r="A24" s="4">
         <v>40804</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1507,7 +1625,7 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="1">
+      <c r="A25" s="4">
         <v>40805</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1524,7 +1642,7 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="1">
+      <c r="A26" s="4">
         <v>40805</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1547,7 +1665,7 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="1">
+      <c r="A27" s="4">
         <v>40823</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1567,7 +1685,7 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="1">
+      <c r="A28" s="4">
         <v>40823</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1587,7 +1705,7 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="1">
+      <c r="A29" s="4">
         <v>40823</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1607,7 +1725,7 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="1">
+      <c r="A30" s="4">
         <v>40823</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1627,7 +1745,7 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="1">
+      <c r="A31" s="4">
         <v>40824</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1647,7 +1765,7 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="1">
+      <c r="A32" s="4">
         <v>40824</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1667,7 +1785,7 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="1">
+      <c r="A33" s="4">
         <v>40824</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1687,7 +1805,7 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="1">
+      <c r="A34" s="4">
         <v>40824</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1707,7 +1825,7 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="1">
+      <c r="A35" s="4">
         <v>40826</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1727,7 +1845,7 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="1">
+      <c r="A36" s="4">
         <v>40826</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1747,7 +1865,7 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="1">
+      <c r="A37" s="4">
         <v>40826</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1767,7 +1885,7 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="1">
+      <c r="A38" s="4">
         <v>40826</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1787,7 +1905,7 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="1">
+      <c r="A39" s="4">
         <v>40827</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -1807,7 +1925,7 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="1">
+      <c r="A40" s="4">
         <v>40827</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1830,7 +1948,7 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="1">
+      <c r="A41" s="4">
         <v>40828</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1850,7 +1968,7 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="1">
+      <c r="A42" s="4">
         <v>40828</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1870,7 +1988,7 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="1">
+      <c r="A43" s="4">
         <v>40828</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1890,7 +2008,7 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="1">
+      <c r="A44" s="4">
         <v>40829</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1910,7 +2028,7 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="1">
+      <c r="A45" s="4">
         <v>40829</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1930,7 +2048,7 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="1">
+      <c r="A46" s="4">
         <v>40829</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -1950,7 +2068,7 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="1">
+      <c r="A47" s="4">
         <v>40829</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -1970,7 +2088,7 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="1">
+      <c r="A48" s="4">
         <v>40830</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -1990,7 +2108,7 @@
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="1">
+      <c r="A49" s="4">
         <v>40830</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2010,7 +2128,7 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="1">
+      <c r="A50" s="4">
         <v>40830</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2030,7 +2148,7 @@
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="1">
+      <c r="A51" s="4">
         <v>40830</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -2047,7 +2165,7 @@
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="1">
+      <c r="A52" s="4">
         <v>40830</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -2067,7 +2185,7 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="1">
+      <c r="A53" s="4">
         <v>40830</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -2084,7 +2202,7 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="1">
+      <c r="A54" s="4">
         <v>40831</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -2104,7 +2222,7 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="1">
+      <c r="A55" s="4">
         <v>40831</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -2124,7 +2242,7 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="1">
+      <c r="A56" s="4">
         <v>40831</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -2144,7 +2262,7 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="1">
+      <c r="A57" s="4">
         <v>40831</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -2164,7 +2282,7 @@
       </c>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="1">
+      <c r="A58" s="4">
         <v>40832</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -2184,7 +2302,7 @@
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="1">
+      <c r="A59" s="4">
         <v>40832</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -2204,7 +2322,7 @@
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="1">
+      <c r="A60" s="4">
         <v>40832</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -2224,7 +2342,7 @@
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="1">
+      <c r="A61" s="4">
         <v>40832</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -2244,7 +2362,7 @@
       </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="1">
+      <c r="A62" s="4">
         <v>40832</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -2264,7 +2382,7 @@
       </c>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="1">
+      <c r="A63" s="4">
         <v>40833</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -2284,7 +2402,7 @@
       </c>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="1">
+      <c r="A64" s="4">
         <v>40833</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -2304,7 +2422,7 @@
       </c>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="1">
+      <c r="A65" s="4">
         <v>40834</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -2324,7 +2442,7 @@
       </c>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="1">
+      <c r="A66" s="4">
         <v>40834</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -2341,7 +2459,7 @@
       </c>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="1">
+      <c r="A67" s="4">
         <v>40834</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -2358,7 +2476,7 @@
       </c>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="1">
+      <c r="A68" s="4">
         <v>40834</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -2378,7 +2496,7 @@
       </c>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" s="1">
+      <c r="A69" s="4">
         <v>40837</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -2398,7 +2516,7 @@
       </c>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" s="1">
+      <c r="A70" s="4">
         <v>40837</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -2418,7 +2536,7 @@
       </c>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="1">
+      <c r="A71" s="4">
         <v>40837</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -2438,7 +2556,7 @@
       </c>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="1">
+      <c r="A72" s="4">
         <v>40837</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -2458,7 +2576,7 @@
       </c>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="1">
+      <c r="A73" s="4">
         <v>40837</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -2475,7 +2593,7 @@
       </c>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="1">
+      <c r="A74" s="4">
         <v>40839</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -2492,7 +2610,7 @@
       </c>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="1">
+      <c r="A75" s="4">
         <v>40839</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -2509,7 +2627,7 @@
       </c>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="1">
+      <c r="A76" s="4">
         <v>40839</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -2526,7 +2644,7 @@
       </c>
     </row>
     <row r="77" spans="1:8">
-      <c r="A77" s="1">
+      <c r="A77" s="4">
         <v>40839</v>
       </c>
       <c r="B77" s="2" t="s">
@@ -2543,7 +2661,7 @@
       </c>
     </row>
     <row r="78" spans="1:8">
-      <c r="A78" s="1">
+      <c r="A78" s="4">
         <v>40840</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -2560,7 +2678,7 @@
       </c>
     </row>
     <row r="79" spans="1:8">
-      <c r="A79" s="1">
+      <c r="A79" s="4">
         <v>40840</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -2583,7 +2701,7 @@
       </c>
     </row>
     <row r="80" spans="1:8">
-      <c r="A80" s="1">
+      <c r="A80" s="4">
         <v>40842</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -2603,7 +2721,7 @@
       </c>
     </row>
     <row r="81" spans="1:8">
-      <c r="A81" s="1">
+      <c r="A81" s="4">
         <v>40842</v>
       </c>
       <c r="B81" s="1" t="s">
@@ -2623,7 +2741,7 @@
       </c>
     </row>
     <row r="82" spans="1:8">
-      <c r="A82" s="1">
+      <c r="A82" s="4">
         <v>40842</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -2643,7 +2761,7 @@
       </c>
     </row>
     <row r="83" spans="1:8">
-      <c r="A83" s="1">
+      <c r="A83" s="4">
         <v>40842</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -2663,7 +2781,7 @@
       </c>
     </row>
     <row r="84" spans="1:8">
-      <c r="A84" s="1">
+      <c r="A84" s="4">
         <v>40843</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -2683,7 +2801,7 @@
       </c>
     </row>
     <row r="85" spans="1:8">
-      <c r="A85" s="1">
+      <c r="A85" s="4">
         <v>40843</v>
       </c>
       <c r="B85" s="1" t="s">
@@ -2703,7 +2821,7 @@
       </c>
     </row>
     <row r="86" spans="1:8">
-      <c r="A86" s="1">
+      <c r="A86" s="4">
         <v>40843</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -2723,7 +2841,7 @@
       </c>
     </row>
     <row r="87" spans="1:8">
-      <c r="A87" s="1">
+      <c r="A87" s="4">
         <v>40843</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -2743,7 +2861,7 @@
       </c>
     </row>
     <row r="88" spans="1:8">
-      <c r="A88" s="1">
+      <c r="A88" s="4">
         <v>40844</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -2763,7 +2881,7 @@
       </c>
     </row>
     <row r="89" spans="1:8">
-      <c r="A89" s="1">
+      <c r="A89" s="4">
         <v>40844</v>
       </c>
       <c r="B89" s="1" t="s">
@@ -2780,7 +2898,7 @@
       </c>
     </row>
     <row r="90" spans="1:8">
-      <c r="A90" s="1">
+      <c r="A90" s="4">
         <v>40844</v>
       </c>
       <c r="B90" s="1" t="s">
@@ -2800,7 +2918,7 @@
       </c>
     </row>
     <row r="91" spans="1:8">
-      <c r="A91" s="1">
+      <c r="A91" s="4">
         <v>40844</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -2820,7 +2938,7 @@
       </c>
     </row>
     <row r="92" spans="1:8">
-      <c r="A92" s="1">
+      <c r="A92" s="4">
         <v>40844</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -2840,7 +2958,7 @@
       </c>
     </row>
     <row r="93" spans="1:8">
-      <c r="A93" s="1">
+      <c r="A93" s="4">
         <v>40844</v>
       </c>
       <c r="B93" s="1" t="s">
@@ -2860,7 +2978,7 @@
       </c>
     </row>
     <row r="94" spans="1:8">
-      <c r="A94" s="1">
+      <c r="A94" s="4">
         <v>40844</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -2877,7 +2995,7 @@
       </c>
     </row>
     <row r="95" spans="1:8">
-      <c r="A95" s="1">
+      <c r="A95" s="4">
         <v>40844</v>
       </c>
       <c r="B95" s="2" t="s">
@@ -2894,7 +3012,7 @@
       </c>
     </row>
     <row r="96" spans="1:8">
-      <c r="A96" s="1">
+      <c r="A96" s="4">
         <v>40847</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -2910,8 +3028,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
-      <c r="A97" s="1">
+    <row r="97" spans="1:8">
+      <c r="A97" s="4">
         <v>40851</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -2927,8 +3045,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
-      <c r="A98" s="1">
+    <row r="98" spans="1:8">
+      <c r="A98" s="4">
         <v>40851</v>
       </c>
       <c r="B98" s="1" t="s">
@@ -2943,9 +3061,12 @@
       <c r="E98" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="99" spans="1:5">
-      <c r="A99" s="1">
+      <c r="H98" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" s="4">
         <v>40853</v>
       </c>
       <c r="B99" s="1" t="s">
@@ -2961,8 +3082,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
-      <c r="A100" s="1">
+    <row r="100" spans="1:8">
+      <c r="A100" s="4">
         <v>40853</v>
       </c>
       <c r="B100" s="2" t="s">
@@ -2978,8 +3099,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
-      <c r="A101" s="1">
+    <row r="101" spans="1:8">
+      <c r="A101" s="4">
         <v>40853</v>
       </c>
       <c r="B101" s="1" t="s">
@@ -2995,8 +3116,8 @@
         <v>130</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
-      <c r="A102" s="1">
+    <row r="102" spans="1:8">
+      <c r="A102" s="4">
         <v>40854</v>
       </c>
       <c r="B102" s="2" t="s">
@@ -3012,8 +3133,8 @@
         <v>135</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
-      <c r="A103" s="1">
+    <row r="103" spans="1:8">
+      <c r="A103" s="4">
         <v>40856</v>
       </c>
       <c r="B103" s="1" t="s">
@@ -3029,8 +3150,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
-      <c r="A104" s="1">
+    <row r="104" spans="1:8">
+      <c r="A104" s="4">
         <v>40856</v>
       </c>
       <c r="B104" s="1" t="s">
@@ -3046,8 +3167,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
-      <c r="A105" s="1">
+    <row r="105" spans="1:8">
+      <c r="A105" s="4">
         <v>40857</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -3063,8 +3184,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
-      <c r="A106" s="1">
+    <row r="106" spans="1:8">
+      <c r="A106" s="4">
         <v>40857</v>
       </c>
       <c r="B106" s="1" t="s">
@@ -3079,9 +3200,12 @@
       <c r="E106" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="107" spans="1:5">
-      <c r="A107" s="1">
+      <c r="H106" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" s="4">
         <v>40858</v>
       </c>
       <c r="B107" s="1" t="s">
@@ -3097,8 +3221,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
-      <c r="A108" s="1">
+    <row r="108" spans="1:8">
+      <c r="A108" s="4">
         <v>40858</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -3114,8 +3238,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
-      <c r="A109" s="1">
+    <row r="109" spans="1:8">
+      <c r="A109" s="4">
         <v>40861</v>
       </c>
       <c r="B109" s="1" t="s">
@@ -3131,8 +3255,8 @@
         <v>140</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
-      <c r="A110" s="1">
+    <row r="110" spans="1:8">
+      <c r="A110" s="4">
         <v>40861</v>
       </c>
       <c r="B110" s="1" t="s">
@@ -3148,8 +3272,8 @@
         <v>141</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
-      <c r="A111" s="1">
+    <row r="111" spans="1:8">
+      <c r="A111" s="4">
         <v>40863</v>
       </c>
       <c r="B111" s="1" t="s">
@@ -3165,8 +3289,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
-      <c r="A112" s="1">
+    <row r="112" spans="1:8">
+      <c r="A112" s="4">
         <v>40863</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -3182,8 +3306,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
-      <c r="A113" s="1">
+    <row r="113" spans="1:8">
+      <c r="A113" s="4">
         <v>40863</v>
       </c>
       <c r="B113" s="1" t="s">
@@ -3199,8 +3323,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
-      <c r="A114" s="1">
+    <row r="114" spans="1:8">
+      <c r="A114" s="4">
         <v>40864</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -3216,8 +3340,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
-      <c r="A115" s="1">
+    <row r="115" spans="1:8">
+      <c r="A115" s="4">
         <v>40864</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -3232,9 +3356,12 @@
       <c r="E115" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="116" spans="1:5">
-      <c r="A116" s="1">
+      <c r="H115" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" s="4">
         <v>40865</v>
       </c>
       <c r="B116" s="1" t="s">
@@ -3250,8 +3377,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
-      <c r="A117" s="1">
+    <row r="117" spans="1:8">
+      <c r="A117" s="4">
         <v>40865</v>
       </c>
       <c r="B117" s="1" t="s">
@@ -3267,8 +3394,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
-      <c r="A118" s="1">
+    <row r="118" spans="1:8">
+      <c r="A118" s="4">
         <v>40868</v>
       </c>
       <c r="B118" s="1" t="s">
@@ -3284,8 +3411,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
-      <c r="A119" s="1">
+    <row r="119" spans="1:8">
+      <c r="A119" s="4">
         <v>40868</v>
       </c>
       <c r="B119" s="1" t="s">
@@ -3301,8 +3428,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
-      <c r="A120" s="1">
+    <row r="120" spans="1:8">
+      <c r="A120" s="4">
         <v>40868</v>
       </c>
       <c r="B120" s="1" t="s">
@@ -3318,25 +3445,25 @@
         <v>152</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
-      <c r="A121" s="1">
+    <row r="121" spans="1:8">
+      <c r="A121" s="4">
         <v>40869</v>
       </c>
       <c r="B121" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C121" t="s">
+        <v>104</v>
+      </c>
+      <c r="D121" t="s">
+        <v>19</v>
+      </c>
+      <c r="E121" t="s">
         <v>153</v>
       </c>
-      <c r="C121" t="s">
-        <v>104</v>
-      </c>
-      <c r="D121" t="s">
-        <v>20</v>
-      </c>
-      <c r="E121" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5">
-      <c r="A122" s="1">
+    </row>
+    <row r="122" spans="1:8">
+      <c r="A122" s="4">
         <v>40869</v>
       </c>
       <c r="B122" s="1" t="s">
@@ -3346,15 +3473,328 @@
         <v>104</v>
       </c>
       <c r="D122" t="s">
+        <v>153</v>
+      </c>
+      <c r="E122" t="s">
         <v>154</v>
       </c>
-      <c r="E122" t="s">
+    </row>
+    <row r="123" spans="1:8">
+      <c r="A123" s="4">
+        <v>40871</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>155</v>
+      </c>
+      <c r="C123" t="s">
+        <v>104</v>
+      </c>
+      <c r="D123" t="s">
+        <v>19</v>
+      </c>
+      <c r="E123" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8">
+      <c r="A124" s="4">
+        <v>40871</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C124" t="s">
+        <v>104</v>
+      </c>
+      <c r="D124" t="s">
+        <v>128</v>
+      </c>
+      <c r="E124" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8">
+      <c r="A125" s="4">
+        <v>40871</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C125" t="s">
+        <v>104</v>
+      </c>
+      <c r="D125" t="s">
+        <v>158</v>
+      </c>
+      <c r="E125" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8">
+      <c r="A126" s="4">
+        <v>40876</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C126" t="s">
+        <v>104</v>
+      </c>
+      <c r="D126" t="s">
+        <v>19</v>
+      </c>
+      <c r="E126" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8">
+      <c r="A127" s="4">
+        <v>40876</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C127" t="s">
+        <v>104</v>
+      </c>
+      <c r="D127" t="s">
+        <v>128</v>
+      </c>
+      <c r="E127" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8">
+      <c r="A128" s="4">
+        <v>40877</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C128" t="s">
+        <v>104</v>
+      </c>
+      <c r="D128" t="s">
+        <v>19</v>
+      </c>
+      <c r="E128" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8">
+      <c r="A129" s="4">
+        <v>40877</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C129" t="s">
+        <v>104</v>
+      </c>
+      <c r="D129" t="s">
+        <v>128</v>
+      </c>
+      <c r="E129" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8">
+      <c r="A130" s="4">
+        <v>40879</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C130" t="s">
+        <v>104</v>
+      </c>
+      <c r="D130" t="s">
+        <v>19</v>
+      </c>
+      <c r="E130" t="s">
+        <v>163</v>
+      </c>
+      <c r="H130" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8">
+      <c r="A131" s="4">
+        <v>40882</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C131" t="s">
+        <v>104</v>
+      </c>
+      <c r="D131" t="s">
+        <v>163</v>
+      </c>
+      <c r="E131" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8">
+      <c r="A132" s="4">
+        <v>40882</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C132" t="s">
+        <v>104</v>
+      </c>
+      <c r="D132" t="s">
+        <v>168</v>
+      </c>
+      <c r="E132" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8">
+      <c r="A133" s="4">
+        <v>40882</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C133" t="s">
+        <v>104</v>
+      </c>
+      <c r="D133" t="s">
+        <v>169</v>
+      </c>
+      <c r="E133" t="s">
+        <v>19</v>
+      </c>
+      <c r="H133" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8">
+      <c r="A134" s="4">
+        <v>40884</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C134" t="s">
+        <v>104</v>
+      </c>
+      <c r="D134" t="s">
+        <v>19</v>
+      </c>
+      <c r="E134" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8">
+      <c r="A135" s="4">
+        <v>40884</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C135" t="s">
+        <v>104</v>
+      </c>
+      <c r="D135" t="s">
+        <v>169</v>
+      </c>
+      <c r="E135" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
+      <c r="A136" s="4">
+        <v>40885</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C136" t="s">
+        <v>104</v>
+      </c>
+      <c r="D136" t="s">
+        <v>19</v>
+      </c>
+      <c r="E136" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8">
+      <c r="A137" s="4">
+        <v>40885</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C137" t="s">
+        <v>104</v>
+      </c>
+      <c r="D137" t="s">
+        <v>169</v>
+      </c>
+      <c r="E137" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8">
+      <c r="A138" s="4">
+        <v>40887</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C138" t="s">
+        <v>104</v>
+      </c>
+      <c r="D138" t="s">
+        <v>57</v>
+      </c>
+      <c r="E138" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8">
+      <c r="A139" s="4">
+        <v>40887</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C139" t="s">
+        <v>104</v>
+      </c>
+      <c r="D139" t="s">
+        <v>169</v>
+      </c>
+      <c r="E139" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8">
+      <c r="A140" s="4">
+        <v>40888</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C140" t="s">
+        <v>104</v>
+      </c>
+      <c r="D140" t="s">
+        <v>177</v>
+      </c>
+      <c r="E140" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
# add xls2cim Template.
</commit_message>
<xml_diff>
--- a/history/drive.xlsx
+++ b/history/drive.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="206">
   <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -849,6 +849,14 @@
   </si>
   <si>
     <t>5:40-8:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+油 ￥40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>违章 -200</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1211,13 +1219,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J151"/>
+  <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C131" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I151" sqref="I151"/>
+      <selection pane="bottomRight" activeCell="G157" sqref="G157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4021,8 +4029,11 @@
         <v>156316</v>
       </c>
       <c r="H146">
-        <f t="shared" ref="H146:H151" si="0">G146-F146</f>
+        <f t="shared" ref="H146:H153" si="0">G146-F146</f>
         <v>125</v>
+      </c>
+      <c r="J146" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="147" spans="1:10">
@@ -4158,6 +4169,63 @@
       <c r="H151">
         <f t="shared" si="0"/>
         <v>108</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10">
+      <c r="A152" s="4">
+        <v>40984</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C152" t="s">
+        <v>103</v>
+      </c>
+      <c r="D152" t="s">
+        <v>19</v>
+      </c>
+      <c r="E152" t="s">
+        <v>47</v>
+      </c>
+      <c r="F152">
+        <v>156714</v>
+      </c>
+      <c r="G152">
+        <v>156829</v>
+      </c>
+      <c r="H152">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10">
+      <c r="A153" s="4">
+        <v>40987</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C153" t="s">
+        <v>103</v>
+      </c>
+      <c r="D153" t="s">
+        <v>47</v>
+      </c>
+      <c r="E153" t="s">
+        <v>19</v>
+      </c>
+      <c r="F153">
+        <v>156848</v>
+      </c>
+      <c r="G153">
+        <v>156955</v>
+      </c>
+      <c r="H153">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+      <c r="J153" s="3" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>